<commit_message>
Big changes today. Still need to resolve a lot of special cases of joints and what to do with link positions (referencePts).
</commit_message>
<xml_diff>
--- a/ExcelPlanarMechSimulator/ExcelPlanarMechSimulator.xlsx
+++ b/ExcelPlanarMechSimulator/ExcelPlanarMechSimulator.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-855" yWindow="3375" windowWidth="20370" windowHeight="7455"/>
+    <workbookView xWindow="-4590" yWindow="-480" windowWidth="14175" windowHeight="11715"/>
   </bookViews>
   <sheets>
     <sheet name="Inputs" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="22">
   <si>
     <t>Describe the Joints of the Mechanism</t>
   </si>
@@ -48,9 +48,6 @@
     <t>r</t>
   </si>
   <si>
-    <t>p</t>
-  </si>
-  <si>
     <t>duet</t>
   </si>
   <si>
@@ -75,13 +72,19 @@
     <t>coupler,block, ac</t>
   </si>
   <si>
-    <t>ac</t>
-  </si>
-  <si>
     <t>ac,output</t>
   </si>
   <si>
     <t>output 0</t>
+  </si>
+  <si>
+    <t>Otto II six bar</t>
+  </si>
+  <si>
+    <t>input coupler</t>
+  </si>
+  <si>
+    <t>coupler,output</t>
   </si>
 </sst>
 </file>
@@ -439,6 +442,27 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -448,29 +472,8 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -777,7 +780,7 @@
   <dimension ref="A1:R22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F26" sqref="F26"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -789,14 +792,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="14"/>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14"/>
-      <c r="E1" s="14"/>
-      <c r="F1" s="15"/>
+      <c r="B1" s="21"/>
+      <c r="C1" s="21"/>
+      <c r="D1" s="21"/>
+      <c r="E1" s="21"/>
+      <c r="F1" s="22"/>
     </row>
     <row r="2" spans="1:18" ht="48.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="10" t="s">
@@ -817,26 +820,26 @@
       <c r="F2" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="H2" s="16" t="s">
+      <c r="H2" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="I2" s="17"/>
-      <c r="J2" s="20" t="s">
+      <c r="I2" s="19"/>
+      <c r="J2" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="K2" s="13"/>
+      <c r="L2" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="K2" s="19"/>
-      <c r="L2" s="16" t="s">
+      <c r="M2" s="19"/>
+      <c r="N2" s="15">
+        <v>1</v>
+      </c>
+      <c r="P2" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="M2" s="17"/>
-      <c r="N2" s="22">
-        <v>1</v>
-      </c>
-      <c r="P2" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="Q2" s="17"/>
-      <c r="R2" s="23">
+      <c r="Q2" s="19"/>
+      <c r="R2" s="16">
         <v>1</v>
       </c>
     </row>
@@ -854,44 +857,44 @@
         <v>0</v>
       </c>
       <c r="E3" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="F3" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="F3" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="H3" s="18"/>
-      <c r="I3" s="18"/>
-      <c r="J3" s="18"/>
-      <c r="K3" s="18"/>
-      <c r="L3" s="18"/>
-      <c r="M3" s="18"/>
+      <c r="H3" s="23"/>
+      <c r="I3" s="23"/>
+      <c r="J3" s="23"/>
+      <c r="K3" s="23"/>
+      <c r="L3" s="23"/>
+      <c r="M3" s="23"/>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>2</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C4" s="3">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="D4" s="3">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="E4" s="3">
         <v>0</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="H4" s="21"/>
-      <c r="I4" s="21"/>
-      <c r="J4" s="21"/>
-      <c r="K4" s="21"/>
-      <c r="L4" s="21"/>
-      <c r="M4" s="21"/>
-      <c r="N4" s="21"/>
+        <v>20</v>
+      </c>
+      <c r="H4" s="17"/>
+      <c r="I4" s="17"/>
+      <c r="J4" s="17"/>
+      <c r="K4" s="17"/>
+      <c r="L4" s="17"/>
+      <c r="M4" s="17"/>
+      <c r="N4" s="17"/>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
@@ -904,21 +907,21 @@
         <v>20</v>
       </c>
       <c r="D5" s="3">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="E5" s="3">
         <v>0</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="H5" s="21"/>
-      <c r="I5" s="21"/>
-      <c r="J5" s="21"/>
-      <c r="K5" s="21"/>
-      <c r="L5" s="21"/>
-      <c r="M5" s="21"/>
-      <c r="N5" s="21"/>
+        <v>21</v>
+      </c>
+      <c r="H5" s="17"/>
+      <c r="I5" s="17"/>
+      <c r="J5" s="17"/>
+      <c r="K5" s="17"/>
+      <c r="L5" s="17"/>
+      <c r="M5" s="17"/>
+      <c r="N5" s="17"/>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
@@ -928,76 +931,52 @@
         <v>8</v>
       </c>
       <c r="C6" s="3">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="D6" s="3">
-        <v>8.5</v>
+        <v>0</v>
       </c>
       <c r="E6" s="3"/>
       <c r="F6" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="H6" s="21"/>
-      <c r="I6" s="21"/>
-      <c r="J6" s="21"/>
-      <c r="K6" s="21"/>
-      <c r="L6" s="21"/>
-      <c r="M6" s="21"/>
-      <c r="N6" s="21"/>
+        <v>18</v>
+      </c>
+      <c r="H6" s="17"/>
+      <c r="I6" s="17"/>
+      <c r="J6" s="17"/>
+      <c r="K6" s="17"/>
+      <c r="L6" s="17"/>
+      <c r="M6" s="17"/>
+      <c r="N6" s="17"/>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>5</v>
       </c>
-      <c r="B7" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C7" s="3">
-        <v>23</v>
-      </c>
-      <c r="D7" s="3">
-        <v>45</v>
-      </c>
+      <c r="B7" s="3"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
       <c r="E7" s="3"/>
-      <c r="F7" s="4" t="s">
-        <v>19</v>
-      </c>
+      <c r="F7" s="4"/>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>6</v>
       </c>
-      <c r="B8" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C8" s="3">
-        <v>67</v>
-      </c>
-      <c r="D8" s="3">
-        <v>78</v>
-      </c>
+      <c r="B8" s="3"/>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
       <c r="E8" s="3"/>
-      <c r="F8" s="4" t="s">
-        <v>20</v>
-      </c>
+      <c r="F8" s="4"/>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>7</v>
       </c>
-      <c r="B9" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C9" s="3">
-        <v>89</v>
-      </c>
-      <c r="D9" s="3">
-        <v>90</v>
-      </c>
+      <c r="B9" s="3"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
       <c r="E9" s="3"/>
-      <c r="F9" s="4" t="s">
-        <v>18</v>
-      </c>
+      <c r="F9" s="4"/>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
@@ -1018,6 +997,9 @@
       <c r="D11" s="3"/>
       <c r="E11" s="3"/>
       <c r="F11" s="4"/>
+      <c r="I11" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
@@ -1028,6 +1010,21 @@
       <c r="D12" s="3"/>
       <c r="E12" s="3"/>
       <c r="F12" s="4"/>
+      <c r="I12" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="J12" s="8">
+        <v>0</v>
+      </c>
+      <c r="K12" s="8">
+        <v>0</v>
+      </c>
+      <c r="L12" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="M12" s="9" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
@@ -1038,6 +1035,21 @@
       <c r="D13" s="3"/>
       <c r="E13" s="3"/>
       <c r="F13" s="4"/>
+      <c r="I13" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="J13" s="3">
+        <v>20</v>
+      </c>
+      <c r="K13" s="3">
+        <v>-10</v>
+      </c>
+      <c r="L13" s="3">
+        <v>0</v>
+      </c>
+      <c r="M13" s="4" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
@@ -1048,6 +1060,21 @@
       <c r="D14" s="3"/>
       <c r="E14" s="3"/>
       <c r="F14" s="4"/>
+      <c r="I14" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="J14" s="3">
+        <v>20</v>
+      </c>
+      <c r="K14" s="3">
+        <v>0</v>
+      </c>
+      <c r="L14" s="3">
+        <v>0</v>
+      </c>
+      <c r="M14" s="4" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
@@ -1058,6 +1085,19 @@
       <c r="D15" s="3"/>
       <c r="E15" s="3"/>
       <c r="F15" s="4"/>
+      <c r="I15" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="J15" s="3">
+        <v>8</v>
+      </c>
+      <c r="K15" s="3">
+        <v>8.5</v>
+      </c>
+      <c r="L15" s="3"/>
+      <c r="M15" s="4" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
@@ -1068,8 +1108,21 @@
       <c r="D16" s="3"/>
       <c r="E16" s="3"/>
       <c r="F16" s="4"/>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I16" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="J16" s="3">
+        <v>23</v>
+      </c>
+      <c r="K16" s="3">
+        <v>45</v>
+      </c>
+      <c r="L16" s="3"/>
+      <c r="M16" s="4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
         <v>15</v>
       </c>
@@ -1078,8 +1131,21 @@
       <c r="D17" s="3"/>
       <c r="E17" s="3"/>
       <c r="F17" s="4"/>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I17" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="J17" s="3">
+        <v>67</v>
+      </c>
+      <c r="K17" s="3">
+        <v>78</v>
+      </c>
+      <c r="L17" s="3"/>
+      <c r="M17" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
         <v>16</v>
       </c>
@@ -1089,7 +1155,7 @@
       <c r="E18" s="3"/>
       <c r="F18" s="4"/>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
         <v>17</v>
       </c>
@@ -1099,7 +1165,7 @@
       <c r="E19" s="3"/>
       <c r="F19" s="4"/>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
         <v>18</v>
       </c>
@@ -1109,7 +1175,7 @@
       <c r="E20" s="3"/>
       <c r="F20" s="4"/>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
         <v>19</v>
       </c>
@@ -1119,7 +1185,7 @@
       <c r="E21" s="3"/>
       <c r="F21" s="4"/>
     </row>
-    <row r="22" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="5">
         <v>20</v>
       </c>
@@ -1132,12 +1198,12 @@
   </sheetData>
   <dataConsolidate/>
   <mergeCells count="6">
+    <mergeCell ref="H4:N6"/>
     <mergeCell ref="P2:Q2"/>
     <mergeCell ref="A1:F1"/>
     <mergeCell ref="H2:I2"/>
     <mergeCell ref="H3:M3"/>
     <mergeCell ref="L2:M2"/>
-    <mergeCell ref="H4:N6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
now showing independent pivots!
</commit_message>
<xml_diff>
--- a/ExcelPlanarMechSimulator/ExcelPlanarMechSimulator.xlsx
+++ b/ExcelPlanarMechSimulator/ExcelPlanarMechSimulator.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-4590" yWindow="-480" windowWidth="14175" windowHeight="11715"/>
+    <workbookView xWindow="-480" yWindow="3375" windowWidth="20010" windowHeight="11205"/>
   </bookViews>
   <sheets>
     <sheet name="Inputs" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="23">
   <si>
     <t>Describe the Joints of the Mechanism</t>
   </si>
@@ -85,6 +85,9 @@
   </si>
   <si>
     <t>coupler,output</t>
+  </si>
+  <si>
+    <t>coupler</t>
   </si>
 </sst>
 </file>
@@ -780,7 +783,7 @@
   <dimension ref="A1:R22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -952,11 +955,19 @@
       <c r="A7" s="2">
         <v>5</v>
       </c>
-      <c r="B7" s="3"/>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
+      <c r="B7" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" s="3">
+        <v>15</v>
+      </c>
+      <c r="D7" s="3">
+        <v>25</v>
+      </c>
       <c r="E7" s="3"/>
-      <c r="F7" s="4"/>
+      <c r="F7" s="4" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8" s="2">

</xml_diff>

<commit_message>
working for R joints! yay.
</commit_message>
<xml_diff>
--- a/ExcelPlanarMechSimulator/ExcelPlanarMechSimulator.xlsx
+++ b/ExcelPlanarMechSimulator/ExcelPlanarMechSimulator.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-480" yWindow="3375" windowWidth="20010" windowHeight="11205"/>
+    <workbookView xWindow="-4590" yWindow="-525" windowWidth="20010" windowHeight="8115"/>
   </bookViews>
   <sheets>
     <sheet name="Inputs" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="26">
   <si>
     <t>Describe the Joints of the Mechanism</t>
   </si>
@@ -87,7 +87,16 @@
     <t>coupler,output</t>
   </si>
   <si>
-    <t>coupler</t>
+    <t>coupler,intermed</t>
+  </si>
+  <si>
+    <t>intermed, gnd</t>
+  </si>
+  <si>
+    <t>intermed, coupler2</t>
+  </si>
+  <si>
+    <t>output, gnd</t>
   </si>
 </sst>
 </file>
@@ -783,7 +792,7 @@
   <dimension ref="A1:R22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -854,7 +863,7 @@
         <v>8</v>
       </c>
       <c r="C3" s="8">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="D3" s="8">
         <v>0</v>
@@ -880,7 +889,7 @@
         <v>8</v>
       </c>
       <c r="C4" s="3">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="D4" s="3">
         <v>10</v>
@@ -910,13 +919,13 @@
         <v>20</v>
       </c>
       <c r="D5" s="3">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="E5" s="3">
         <v>0</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H5" s="17"/>
       <c r="I5" s="17"/>
@@ -941,7 +950,7 @@
       </c>
       <c r="E6" s="3"/>
       <c r="F6" s="4" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="H6" s="17"/>
       <c r="I6" s="17"/>
@@ -959,35 +968,51 @@
         <v>8</v>
       </c>
       <c r="C7" s="3">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="D7" s="3">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="E7" s="3"/>
       <c r="F7" s="4" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>6</v>
       </c>
-      <c r="B8" s="3"/>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
+      <c r="B8" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" s="3">
+        <v>0</v>
+      </c>
+      <c r="D8" s="3">
+        <v>20</v>
+      </c>
       <c r="E8" s="3"/>
-      <c r="F8" s="4"/>
+      <c r="F8" s="4" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>7</v>
       </c>
-      <c r="B9" s="3"/>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
+      <c r="B9" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C9" s="3">
+        <v>0</v>
+      </c>
+      <c r="D9" s="3">
+        <v>0</v>
+      </c>
       <c r="E9" s="3"/>
-      <c r="F9" s="4"/>
+      <c r="F9" s="4" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10" s="2">

</xml_diff>

<commit_message>
big changes. I got the non-dyadic working. double-butterfly madness!!
</commit_message>
<xml_diff>
--- a/ExcelPlanarMechSimulator/ExcelPlanarMechSimulator.xlsx
+++ b/ExcelPlanarMechSimulator/ExcelPlanarMechSimulator.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-4590" yWindow="-525" windowWidth="20010" windowHeight="8115"/>
+    <workbookView xWindow="465" yWindow="2700" windowWidth="15135" windowHeight="6435"/>
   </bookViews>
   <sheets>
     <sheet name="Inputs" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="30">
   <si>
     <t>Describe the Joints of the Mechanism</t>
   </si>
@@ -54,12 +54,6 @@
     <t>input gnd</t>
   </si>
   <si>
-    <t>ground block</t>
-  </si>
-  <si>
-    <t>input, coupler</t>
-  </si>
-  <si>
     <t>?</t>
   </si>
   <si>
@@ -69,24 +63,12 @@
     <t>Angle Increment:</t>
   </si>
   <si>
-    <t>coupler,block, ac</t>
-  </si>
-  <si>
-    <t>ac,output</t>
-  </si>
-  <si>
-    <t>output 0</t>
-  </si>
-  <si>
     <t>Otto II six bar</t>
   </si>
   <si>
     <t>input coupler</t>
   </si>
   <si>
-    <t>coupler,output</t>
-  </si>
-  <si>
     <t>coupler,intermed</t>
   </si>
   <si>
@@ -97,6 +79,36 @@
   </si>
   <si>
     <t>output, gnd</t>
+  </si>
+  <si>
+    <t>coupler2,output</t>
+  </si>
+  <si>
+    <t>input, up1</t>
+  </si>
+  <si>
+    <t>input, up2</t>
+  </si>
+  <si>
+    <t>up1, wing1</t>
+  </si>
+  <si>
+    <t>up2,wing2</t>
+  </si>
+  <si>
+    <t>wing1, wing2</t>
+  </si>
+  <si>
+    <t>wing1,leg1</t>
+  </si>
+  <si>
+    <t>wing2,leg2</t>
+  </si>
+  <si>
+    <t>leg2, gnd</t>
+  </si>
+  <si>
+    <t>leg1, gnd</t>
   </si>
 </sst>
 </file>
@@ -179,7 +191,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="20">
+  <borders count="22">
     <border>
       <left/>
       <right/>
@@ -432,11 +444,33 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="hair">
+        <color indexed="64"/>
+      </left>
+      <right style="hair">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="hair">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
@@ -466,9 +500,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -487,6 +518,11 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -791,8 +827,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:R22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView tabSelected="1" topLeftCell="I5" workbookViewId="0">
+      <selection activeCell="I22" sqref="I22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -804,14 +840,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="21"/>
-      <c r="C1" s="21"/>
-      <c r="D1" s="21"/>
-      <c r="E1" s="21"/>
-      <c r="F1" s="22"/>
+      <c r="B1" s="20"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
+      <c r="F1" s="21"/>
     </row>
     <row r="2" spans="1:18" ht="48.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="10" t="s">
@@ -832,25 +868,25 @@
       <c r="F2" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="H2" s="18" t="s">
+      <c r="H2" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="I2" s="19"/>
+      <c r="I2" s="18"/>
       <c r="J2" s="14" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="K2" s="13"/>
-      <c r="L2" s="18" t="s">
-        <v>14</v>
-      </c>
-      <c r="M2" s="19"/>
+      <c r="L2" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="M2" s="18"/>
       <c r="N2" s="15">
         <v>1</v>
       </c>
-      <c r="P2" s="18" t="s">
-        <v>15</v>
-      </c>
-      <c r="Q2" s="19"/>
+      <c r="P2" s="17" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q2" s="18"/>
       <c r="R2" s="16">
         <v>1</v>
       </c>
@@ -874,12 +910,12 @@
       <c r="F3" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="H3" s="23"/>
-      <c r="I3" s="23"/>
-      <c r="J3" s="23"/>
-      <c r="K3" s="23"/>
-      <c r="L3" s="23"/>
-      <c r="M3" s="23"/>
+      <c r="H3" s="22"/>
+      <c r="I3" s="22"/>
+      <c r="J3" s="22"/>
+      <c r="K3" s="22"/>
+      <c r="L3" s="22"/>
+      <c r="M3" s="22"/>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
@@ -892,21 +928,21 @@
         <v>30</v>
       </c>
       <c r="D4" s="3">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E4" s="3">
         <v>0</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="H4" s="17"/>
-      <c r="I4" s="17"/>
-      <c r="J4" s="17"/>
-      <c r="K4" s="17"/>
-      <c r="L4" s="17"/>
-      <c r="M4" s="17"/>
-      <c r="N4" s="17"/>
+        <v>15</v>
+      </c>
+      <c r="H4" s="23"/>
+      <c r="I4" s="23"/>
+      <c r="J4" s="23"/>
+      <c r="K4" s="23"/>
+      <c r="L4" s="23"/>
+      <c r="M4" s="23"/>
+      <c r="N4" s="23"/>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
@@ -925,15 +961,15 @@
         <v>0</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="H5" s="17"/>
-      <c r="I5" s="17"/>
-      <c r="J5" s="17"/>
-      <c r="K5" s="17"/>
-      <c r="L5" s="17"/>
-      <c r="M5" s="17"/>
-      <c r="N5" s="17"/>
+        <v>16</v>
+      </c>
+      <c r="H5" s="23"/>
+      <c r="I5" s="23"/>
+      <c r="J5" s="23"/>
+      <c r="K5" s="23"/>
+      <c r="L5" s="23"/>
+      <c r="M5" s="23"/>
+      <c r="N5" s="23"/>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
@@ -950,15 +986,15 @@
       </c>
       <c r="E6" s="3"/>
       <c r="F6" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="H6" s="17"/>
-      <c r="I6" s="17"/>
-      <c r="J6" s="17"/>
-      <c r="K6" s="17"/>
-      <c r="L6" s="17"/>
-      <c r="M6" s="17"/>
-      <c r="N6" s="17"/>
+        <v>17</v>
+      </c>
+      <c r="H6" s="23"/>
+      <c r="I6" s="23"/>
+      <c r="J6" s="23"/>
+      <c r="K6" s="23"/>
+      <c r="L6" s="23"/>
+      <c r="M6" s="23"/>
+      <c r="N6" s="23"/>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
@@ -971,12 +1007,19 @@
         <v>20</v>
       </c>
       <c r="D7" s="3">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E7" s="3"/>
       <c r="F7" s="4" t="s">
-        <v>24</v>
-      </c>
+        <v>18</v>
+      </c>
+      <c r="H7" s="23"/>
+      <c r="I7" s="23"/>
+      <c r="J7" s="23"/>
+      <c r="K7" s="23"/>
+      <c r="L7" s="23"/>
+      <c r="M7" s="23"/>
+      <c r="N7" s="23"/>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
@@ -993,8 +1036,15 @@
       </c>
       <c r="E8" s="3"/>
       <c r="F8" s="4" t="s">
-        <v>21</v>
-      </c>
+        <v>20</v>
+      </c>
+      <c r="H8" s="23"/>
+      <c r="I8" s="23"/>
+      <c r="J8" s="23"/>
+      <c r="K8" s="23"/>
+      <c r="L8" s="23"/>
+      <c r="M8" s="23"/>
+      <c r="N8" s="23"/>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
@@ -1011,8 +1061,15 @@
       </c>
       <c r="E9" s="3"/>
       <c r="F9" s="4" t="s">
-        <v>25</v>
-      </c>
+        <v>19</v>
+      </c>
+      <c r="H9" s="23"/>
+      <c r="I9" s="23"/>
+      <c r="J9" s="23"/>
+      <c r="K9" s="23"/>
+      <c r="L9" s="23"/>
+      <c r="M9" s="23"/>
+      <c r="N9" s="23"/>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
@@ -1034,7 +1091,7 @@
       <c r="E11" s="3"/>
       <c r="F11" s="4"/>
       <c r="I11" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.25">
@@ -1055,9 +1112,7 @@
       <c r="K12" s="8">
         <v>0</v>
       </c>
-      <c r="L12" s="8" t="s">
-        <v>9</v>
-      </c>
+      <c r="L12" s="8"/>
       <c r="M12" s="9" t="s">
         <v>10</v>
       </c>
@@ -1075,16 +1130,16 @@
         <v>8</v>
       </c>
       <c r="J13" s="3">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="K13" s="3">
-        <v>-10</v>
+        <v>4</v>
       </c>
       <c r="L13" s="3">
         <v>0</v>
       </c>
       <c r="M13" s="4" t="s">
-        <v>11</v>
+        <v>21</v>
       </c>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.25">
@@ -1100,16 +1155,16 @@
         <v>8</v>
       </c>
       <c r="J14" s="3">
-        <v>20</v>
+        <v>-4</v>
       </c>
       <c r="K14" s="3">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="L14" s="3">
         <v>0</v>
       </c>
       <c r="M14" s="4" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.25">
@@ -1125,14 +1180,14 @@
         <v>8</v>
       </c>
       <c r="J15" s="3">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="K15" s="3">
-        <v>8.5</v>
+        <v>10</v>
       </c>
       <c r="L15" s="3"/>
       <c r="M15" s="4" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.25">
@@ -1148,14 +1203,14 @@
         <v>8</v>
       </c>
       <c r="J16" s="3">
-        <v>23</v>
+        <v>-4</v>
       </c>
       <c r="K16" s="3">
-        <v>45</v>
+        <v>10</v>
       </c>
       <c r="L16" s="3"/>
       <c r="M16" s="4" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.25">
@@ -1171,14 +1226,14 @@
         <v>8</v>
       </c>
       <c r="J17" s="3">
-        <v>67</v>
+        <v>0</v>
       </c>
       <c r="K17" s="3">
-        <v>78</v>
+        <v>13</v>
       </c>
       <c r="L17" s="3"/>
       <c r="M17" s="4" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.25">
@@ -1190,6 +1245,18 @@
       <c r="D18" s="3"/>
       <c r="E18" s="3"/>
       <c r="F18" s="4"/>
+      <c r="I18" s="24" t="s">
+        <v>8</v>
+      </c>
+      <c r="J18" s="24">
+        <v>6</v>
+      </c>
+      <c r="K18" s="24">
+        <v>13</v>
+      </c>
+      <c r="M18" s="25" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
@@ -1200,6 +1267,18 @@
       <c r="D19" s="3"/>
       <c r="E19" s="3"/>
       <c r="F19" s="4"/>
+      <c r="I19" s="24" t="s">
+        <v>8</v>
+      </c>
+      <c r="J19" s="24">
+        <v>-6</v>
+      </c>
+      <c r="K19" s="24">
+        <v>13</v>
+      </c>
+      <c r="M19" s="25" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
@@ -1210,6 +1289,18 @@
       <c r="D20" s="3"/>
       <c r="E20" s="3"/>
       <c r="F20" s="4"/>
+      <c r="I20" s="24" t="s">
+        <v>8</v>
+      </c>
+      <c r="J20" s="24">
+        <v>-6</v>
+      </c>
+      <c r="K20" s="24">
+        <v>-4</v>
+      </c>
+      <c r="M20" s="25" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
@@ -1220,6 +1311,18 @@
       <c r="D21" s="3"/>
       <c r="E21" s="3"/>
       <c r="F21" s="4"/>
+      <c r="I21" s="24" t="s">
+        <v>8</v>
+      </c>
+      <c r="J21" s="24">
+        <v>6</v>
+      </c>
+      <c r="K21" s="24">
+        <v>-4</v>
+      </c>
+      <c r="M21" s="25" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="22" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="5">
@@ -1234,12 +1337,12 @@
   </sheetData>
   <dataConsolidate/>
   <mergeCells count="6">
-    <mergeCell ref="H4:N6"/>
     <mergeCell ref="P2:Q2"/>
     <mergeCell ref="A1:F1"/>
     <mergeCell ref="H2:I2"/>
     <mergeCell ref="H3:M3"/>
     <mergeCell ref="L2:M2"/>
+    <mergeCell ref="H4:N9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
got it running with P's - still some strange behaviors
</commit_message>
<xml_diff>
--- a/ExcelPlanarMechSimulator/ExcelPlanarMechSimulator.xlsx
+++ b/ExcelPlanarMechSimulator/ExcelPlanarMechSimulator.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="465" yWindow="2700" windowWidth="15135" windowHeight="6435"/>
+    <workbookView xWindow="-4590" yWindow="1860" windowWidth="18705" windowHeight="11205"/>
   </bookViews>
   <sheets>
     <sheet name="Inputs" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="35">
   <si>
     <t>Describe the Joints of the Mechanism</t>
   </si>
@@ -109,6 +109,21 @@
   </si>
   <si>
     <t>leg1, gnd</t>
+  </si>
+  <si>
+    <t>Crank and slider</t>
+  </si>
+  <si>
+    <t>p</t>
+  </si>
+  <si>
+    <t>gnd input</t>
+  </si>
+  <si>
+    <t>coupler output</t>
+  </si>
+  <si>
+    <t>output gnd</t>
   </si>
 </sst>
 </file>
@@ -500,6 +515,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -521,8 +538,6 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -825,10 +840,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:R22"/>
+  <dimension ref="A1:R30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I5" workbookViewId="0">
-      <selection activeCell="I22" sqref="I22"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="G28" sqref="G28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -840,14 +855,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="19" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="20"/>
-      <c r="C1" s="20"/>
-      <c r="D1" s="20"/>
-      <c r="E1" s="20"/>
-      <c r="F1" s="21"/>
+      <c r="A1" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="23"/>
     </row>
     <row r="2" spans="1:18" ht="48.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="10" t="s">
@@ -868,25 +883,25 @@
       <c r="F2" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="H2" s="17" t="s">
+      <c r="H2" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="I2" s="18"/>
+      <c r="I2" s="20"/>
       <c r="J2" s="14" t="s">
         <v>11</v>
       </c>
       <c r="K2" s="13"/>
-      <c r="L2" s="17" t="s">
+      <c r="L2" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="M2" s="18"/>
+      <c r="M2" s="20"/>
       <c r="N2" s="15">
         <v>1</v>
       </c>
-      <c r="P2" s="17" t="s">
+      <c r="P2" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="Q2" s="18"/>
+      <c r="Q2" s="20"/>
       <c r="R2" s="16">
         <v>1</v>
       </c>
@@ -910,12 +925,12 @@
       <c r="F3" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="H3" s="22"/>
-      <c r="I3" s="22"/>
-      <c r="J3" s="22"/>
-      <c r="K3" s="22"/>
-      <c r="L3" s="22"/>
-      <c r="M3" s="22"/>
+      <c r="H3" s="24"/>
+      <c r="I3" s="24"/>
+      <c r="J3" s="24"/>
+      <c r="K3" s="24"/>
+      <c r="L3" s="24"/>
+      <c r="M3" s="24"/>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
@@ -936,13 +951,13 @@
       <c r="F4" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="H4" s="23"/>
-      <c r="I4" s="23"/>
-      <c r="J4" s="23"/>
-      <c r="K4" s="23"/>
-      <c r="L4" s="23"/>
-      <c r="M4" s="23"/>
-      <c r="N4" s="23"/>
+      <c r="H4" s="25"/>
+      <c r="I4" s="25"/>
+      <c r="J4" s="25"/>
+      <c r="K4" s="25"/>
+      <c r="L4" s="25"/>
+      <c r="M4" s="25"/>
+      <c r="N4" s="25"/>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
@@ -963,13 +978,13 @@
       <c r="F5" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="H5" s="23"/>
-      <c r="I5" s="23"/>
-      <c r="J5" s="23"/>
-      <c r="K5" s="23"/>
-      <c r="L5" s="23"/>
-      <c r="M5" s="23"/>
-      <c r="N5" s="23"/>
+      <c r="H5" s="25"/>
+      <c r="I5" s="25"/>
+      <c r="J5" s="25"/>
+      <c r="K5" s="25"/>
+      <c r="L5" s="25"/>
+      <c r="M5" s="25"/>
+      <c r="N5" s="25"/>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
@@ -988,13 +1003,13 @@
       <c r="F6" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="H6" s="23"/>
-      <c r="I6" s="23"/>
-      <c r="J6" s="23"/>
-      <c r="K6" s="23"/>
-      <c r="L6" s="23"/>
-      <c r="M6" s="23"/>
-      <c r="N6" s="23"/>
+      <c r="H6" s="25"/>
+      <c r="I6" s="25"/>
+      <c r="J6" s="25"/>
+      <c r="K6" s="25"/>
+      <c r="L6" s="25"/>
+      <c r="M6" s="25"/>
+      <c r="N6" s="25"/>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
@@ -1013,13 +1028,13 @@
       <c r="F7" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="H7" s="23"/>
-      <c r="I7" s="23"/>
-      <c r="J7" s="23"/>
-      <c r="K7" s="23"/>
-      <c r="L7" s="23"/>
-      <c r="M7" s="23"/>
-      <c r="N7" s="23"/>
+      <c r="H7" s="25"/>
+      <c r="I7" s="25"/>
+      <c r="J7" s="25"/>
+      <c r="K7" s="25"/>
+      <c r="L7" s="25"/>
+      <c r="M7" s="25"/>
+      <c r="N7" s="25"/>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
@@ -1038,13 +1053,13 @@
       <c r="F8" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="H8" s="23"/>
-      <c r="I8" s="23"/>
-      <c r="J8" s="23"/>
-      <c r="K8" s="23"/>
-      <c r="L8" s="23"/>
-      <c r="M8" s="23"/>
-      <c r="N8" s="23"/>
+      <c r="H8" s="25"/>
+      <c r="I8" s="25"/>
+      <c r="J8" s="25"/>
+      <c r="K8" s="25"/>
+      <c r="L8" s="25"/>
+      <c r="M8" s="25"/>
+      <c r="N8" s="25"/>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
@@ -1063,13 +1078,13 @@
       <c r="F9" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="H9" s="23"/>
-      <c r="I9" s="23"/>
-      <c r="J9" s="23"/>
-      <c r="K9" s="23"/>
-      <c r="L9" s="23"/>
-      <c r="M9" s="23"/>
-      <c r="N9" s="23"/>
+      <c r="H9" s="25"/>
+      <c r="I9" s="25"/>
+      <c r="J9" s="25"/>
+      <c r="K9" s="25"/>
+      <c r="L9" s="25"/>
+      <c r="M9" s="25"/>
+      <c r="N9" s="25"/>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
@@ -1245,16 +1260,16 @@
       <c r="D18" s="3"/>
       <c r="E18" s="3"/>
       <c r="F18" s="4"/>
-      <c r="I18" s="24" t="s">
-        <v>8</v>
-      </c>
-      <c r="J18" s="24">
+      <c r="I18" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="J18" s="17">
         <v>6</v>
       </c>
-      <c r="K18" s="24">
+      <c r="K18" s="17">
         <v>13</v>
       </c>
-      <c r="M18" s="25" t="s">
+      <c r="M18" s="18" t="s">
         <v>26</v>
       </c>
     </row>
@@ -1267,16 +1282,16 @@
       <c r="D19" s="3"/>
       <c r="E19" s="3"/>
       <c r="F19" s="4"/>
-      <c r="I19" s="24" t="s">
-        <v>8</v>
-      </c>
-      <c r="J19" s="24">
+      <c r="I19" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="J19" s="17">
         <v>-6</v>
       </c>
-      <c r="K19" s="24">
+      <c r="K19" s="17">
         <v>13</v>
       </c>
-      <c r="M19" s="25" t="s">
+      <c r="M19" s="18" t="s">
         <v>27</v>
       </c>
     </row>
@@ -1289,16 +1304,16 @@
       <c r="D20" s="3"/>
       <c r="E20" s="3"/>
       <c r="F20" s="4"/>
-      <c r="I20" s="24" t="s">
-        <v>8</v>
-      </c>
-      <c r="J20" s="24">
+      <c r="I20" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="J20" s="17">
         <v>-6</v>
       </c>
-      <c r="K20" s="24">
+      <c r="K20" s="17">
         <v>-4</v>
       </c>
-      <c r="M20" s="25" t="s">
+      <c r="M20" s="18" t="s">
         <v>28</v>
       </c>
     </row>
@@ -1311,16 +1326,16 @@
       <c r="D21" s="3"/>
       <c r="E21" s="3"/>
       <c r="F21" s="4"/>
-      <c r="I21" s="24" t="s">
-        <v>8</v>
-      </c>
-      <c r="J21" s="24">
+      <c r="I21" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="J21" s="17">
         <v>6</v>
       </c>
-      <c r="K21" s="24">
+      <c r="K21" s="17">
         <v>-4</v>
       </c>
-      <c r="M21" s="25" t="s">
+      <c r="M21" s="18" t="s">
         <v>29</v>
       </c>
     </row>
@@ -1334,15 +1349,79 @@
       <c r="E22" s="6"/>
       <c r="F22" s="7"/>
     </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B26" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B27" t="s">
+        <v>8</v>
+      </c>
+      <c r="C27">
+        <v>0</v>
+      </c>
+      <c r="D27">
+        <v>0</v>
+      </c>
+      <c r="F27" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B28" t="s">
+        <v>8</v>
+      </c>
+      <c r="C28">
+        <v>0</v>
+      </c>
+      <c r="D28">
+        <v>5</v>
+      </c>
+      <c r="F28" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B29" t="s">
+        <v>31</v>
+      </c>
+      <c r="C29">
+        <v>10</v>
+      </c>
+      <c r="D29">
+        <v>8</v>
+      </c>
+      <c r="E29">
+        <v>45</v>
+      </c>
+      <c r="F29" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B30" t="s">
+        <v>8</v>
+      </c>
+      <c r="C30">
+        <v>9</v>
+      </c>
+      <c r="D30">
+        <v>0</v>
+      </c>
+      <c r="F30" t="s">
+        <v>34</v>
+      </c>
+    </row>
   </sheetData>
   <dataConsolidate/>
   <mergeCells count="6">
+    <mergeCell ref="H4:N9"/>
     <mergeCell ref="P2:Q2"/>
     <mergeCell ref="A1:F1"/>
     <mergeCell ref="H2:I2"/>
     <mergeCell ref="H3:M3"/>
     <mergeCell ref="L2:M2"/>
-    <mergeCell ref="H4:N9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>